<commit_message>
Finalized ESC table, improved wireless documentation
</commit_message>
<xml_diff>
--- a/sedani/Sedani PWM Table.xlsx
+++ b/sedani/Sedani PWM Table.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jspall16/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jspall16/Documents/GitHub/roboracing-firmware/sedani/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780D8752-2F92-BF43-873D-09D6CCFCDC8F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449ADB61-3034-7D49-AB93-7C36C0A8CBA2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="3280" windowWidth="28040" windowHeight="16240" xr2:uid="{6F314FEB-716F-9A4B-A55B-0CA5F193E4E1}"/>
+    <workbookView xWindow="7700" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{6F314FEB-716F-9A4B-A55B-0CA5F193E4E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -89,6 +89,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PWM vs Velocity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40671522309711289"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -160,14 +193,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="7.0910979877515309E-2"/>
-                  <c:y val="-0.72471201516477102"/>
+                  <c:x val="0.13252513247164852"/>
+                  <c:y val="-0.17171296296296296"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -202,90 +235,174 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$15</c:f>
+              <c:f>Sheet1!$A$1:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0.42016806722689076</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41841004184100422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43103448275862072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51813471502590669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51813471502590669</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54644808743169393</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54644808743169393</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57803468208092479</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.75987841945288748</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>0.78431372549019618</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="10">
                   <c:v>0.81900081900081889</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>1.4084507042253522</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>1.3869625520110958</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>1.3736263736263736</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>1.9230769230769229</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
                   <c:v>1.8214936247723132</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>1.9157088122605364</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
                   <c:v>2.4752475247524752</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="18">
                   <c:v>2.4096385542168672</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="19">
                   <c:v>2.3923444976076556</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.3255813953488373</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2727272727272725</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.6315789473684212</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.6315789473684212</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.6315789473684212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$15</c:f>
+              <c:f>Sheet1!$B$1:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1533</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1533</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1533</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1533</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1543</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>1543</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="10">
                   <c:v>1543</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>1553</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>1553</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>1553</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>1563</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
                   <c:v>1563</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>1563</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
                   <c:v>1573</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="18">
                   <c:v>1573</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="19">
                   <c:v>1573</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1573</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1573</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1573</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1583</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1583</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,7 +601,457 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PWM</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Velocity Aver</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15946128608923885"/>
+                  <c:y val="-0.17634259259259261"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.42320419727550523</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54144005739922518</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7877309879813007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3896798766209404</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8867597867032575</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3496269111458883</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6315789473684212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1533</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1543</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1553</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1563</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1573</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1583</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2376-CE44-8B07-CEBB8046C6ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2101985871"/>
+        <c:axId val="2101987551"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2101985871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2101987551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2101987551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2101985871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1040,20 +1607,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1073,6 +2156,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8821E432-3A17-8C44-9F82-0B073189C5ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1378,137 +2497,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13803800-E6EB-C148-B3A1-6E9FFB23D01D}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
+        <v>0.42016806722689076</v>
+      </c>
+      <c r="B1">
+        <v>1523</v>
+      </c>
+      <c r="D1">
+        <f>AVERAGE(A1:A3)</f>
+        <v>0.42320419727550523</v>
+      </c>
+      <c r="E1">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.41841004184100422</v>
+      </c>
+      <c r="B2">
+        <v>1523</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(A4:A8)</f>
+        <v>0.54144005739922518</v>
+      </c>
+      <c r="E2">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.43103448275862072</v>
+      </c>
+      <c r="B3">
+        <v>1523</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(A9:A11)</f>
+        <v>0.7877309879813007</v>
+      </c>
+      <c r="E3">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.51813471502590669</v>
+      </c>
+      <c r="B4">
+        <v>1533</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGE(A12:A14)</f>
+        <v>1.3896798766209404</v>
+      </c>
+      <c r="E4">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.51813471502590669</v>
+      </c>
+      <c r="B5">
+        <v>1533</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGE(A15:A17)</f>
+        <v>1.8867597867032575</v>
+      </c>
+      <c r="E5">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.54644808743169393</v>
+      </c>
+      <c r="B6">
+        <v>1533</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE(A18:A23)</f>
+        <v>2.3496269111458883</v>
+      </c>
+      <c r="E6">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.54644808743169393</v>
+      </c>
+      <c r="B7">
+        <v>1533</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE(A24:A26)</f>
+        <v>2.6315789473684212</v>
+      </c>
+      <c r="E7">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.57803468208092479</v>
+      </c>
+      <c r="B8">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>0.75987841945288748</v>
       </c>
-      <c r="B1">
+      <c r="B9">
         <v>1543</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>0.78431372549019618</v>
       </c>
-      <c r="B2">
+      <c r="B10">
         <v>1543</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>0.81900081900081889</v>
       </c>
-      <c r="B3">
+      <c r="B11">
         <v>1543</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>1.4084507042253522</v>
       </c>
-      <c r="B4">
+      <c r="B12">
         <v>1553</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>1.3869625520110958</v>
       </c>
-      <c r="B5">
+      <c r="B13">
         <v>1553</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>1.3736263736263736</v>
       </c>
-      <c r="B6">
+      <c r="B14">
         <v>1553</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>1.9230769230769229</v>
       </c>
-      <c r="B7">
+      <c r="B15">
         <v>1563</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>1.8214936247723132</v>
       </c>
-      <c r="B8">
+      <c r="B16">
         <v>1563</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>1.9157088122605364</v>
       </c>
-      <c r="B9">
+      <c r="B17">
         <v>1563</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>2.4752475247524752</v>
       </c>
-      <c r="B10">
+      <c r="B18">
         <v>1573</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>2.4096385542168672</v>
       </c>
-      <c r="B11">
+      <c r="B19">
         <v>1573</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>2.3923444976076556</v>
       </c>
-      <c r="B12">
+      <c r="B20">
         <v>1573</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1463</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2.3255813953488373</v>
+      </c>
+      <c r="B21">
+        <v>1573</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1463</v>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2.2727272727272725</v>
+      </c>
+      <c r="B22">
+        <v>1573</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1463</v>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="B23">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2.6315789473684212</v>
+      </c>
+      <c r="B24">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2.6315789473684212</v>
+      </c>
+      <c r="B25">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2.6315789473684212</v>
+      </c>
+      <c r="B26">
+        <v>1583</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B12">
-    <sortCondition ref="A1"/>
+  <sortState ref="A1:B26">
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>